<commit_message>
update 3 for reqs section
</commit_message>
<xml_diff>
--- a/Reports/proposal_report/objective_tree.xlsx
+++ b/Reports/proposal_report/objective_tree.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Halil Temurtaş\Desktop\Ekstra\Capstone_Duayenler\Reports\proposal_report\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F8EFEEB-9D0A-450E-8C4D-2A0FDD639E50}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{201D37B1-1B40-44C0-94D0-CA6896C65459}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -78,9 +78,6 @@
     <t>Chasing Cars</t>
   </si>
   <si>
-    <t>Mapping</t>
-  </si>
-  <si>
     <t>Competition</t>
   </si>
   <si>
@@ -130,9 +127,6 @@
     <t>Integration to Auto.</t>
   </si>
   <si>
-    <t>Balloon</t>
-  </si>
-  <si>
     <t>Mechanical Challenges  
 (0.12)</t>
   </si>
@@ -147,10 +141,6 @@
 (0.14)</t>
   </si>
   <si>
-    <t>Robust and Relaible Operation
-(0.14)</t>
-  </si>
-  <si>
     <t>Weight Balance
 (0.17)</t>
   </si>
@@ -175,35 +165,48 @@
 (0.11)</t>
   </si>
   <si>
-    <t>Integreation to Autonomous Systems
+    <t>Design 1</t>
+  </si>
+  <si>
+    <t>Design 2</t>
+  </si>
+  <si>
+    <t>Design 3</t>
+  </si>
+  <si>
+    <t>10: Excellent</t>
+  </si>
+  <si>
+    <t>8: Good</t>
+  </si>
+  <si>
+    <t>2: Unacceptable</t>
+  </si>
+  <si>
+    <t>0: Failure</t>
+  </si>
+  <si>
+    <t>4: Average</t>
+  </si>
+  <si>
+    <t>6: Satisfactory</t>
+  </si>
+  <si>
+    <t>Robust and Reliable  
+Operation
+(0.14)</t>
+  </si>
+  <si>
+    <t>Integration to Autonomous Systems
 (0.09)</t>
   </si>
   <si>
-    <t>Design 1</t>
-  </si>
-  <si>
-    <t>Design 2</t>
-  </si>
-  <si>
-    <t>Design 3</t>
-  </si>
-  <si>
-    <t>10: Excellent</t>
-  </si>
-  <si>
-    <t>8: Good</t>
-  </si>
-  <si>
-    <t>2: Unacceptable</t>
-  </si>
-  <si>
-    <t>0: Failure</t>
-  </si>
-  <si>
-    <t>4: Average</t>
-  </si>
-  <si>
-    <t>6: Satisfactory</t>
+    <t>Balloon
+Catching</t>
+  </si>
+  <si>
+    <t>Mapping
+Robot</t>
   </si>
 </sst>
 </file>
@@ -386,7 +389,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -504,6 +507,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -828,8 +837,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,7 +853,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>1</v>
@@ -853,7 +862,7 @@
         <v>2</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>3</v>
@@ -903,7 +912,7 @@
     </row>
     <row r="4" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C4" s="7">
         <v>0.5</v>
@@ -1002,7 +1011,7 @@
     </row>
     <row r="7" spans="2:11" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C7" s="4">
         <v>0.1</v>
@@ -1124,7 +1133,7 @@
         <v>7</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>11</v>
@@ -1133,7 +1142,7 @@
         <v>8</v>
       </c>
       <c r="G13" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H13" s="11" t="s">
         <v>9</v>
@@ -1146,8 +1155,8 @@
       </c>
     </row>
     <row r="14" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="33" t="s">
-        <v>31</v>
+      <c r="B14" s="42" t="s">
+        <v>51</v>
       </c>
       <c r="C14" s="14">
         <v>8</v>
@@ -1209,7 +1218,7 @@
     </row>
     <row r="16" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="35" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" s="7">
         <v>8</v>
@@ -1332,8 +1341,8 @@
       <c r="J19" s="38"/>
     </row>
     <row r="20" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
-        <v>14</v>
+      <c r="B20" s="43" t="s">
+        <v>52</v>
       </c>
       <c r="C20" s="7">
         <v>4</v>
@@ -1397,16 +1406,16 @@
     <row r="24" spans="1:10" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B24" s="1"/>
       <c r="C24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="2" t="s">
+      <c r="E24" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F24" s="2" t="s">
         <v>19</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F24" s="2" t="s">
-        <v>20</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>5</v>
@@ -1417,7 +1426,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C25" s="4">
         <v>0</v>
@@ -1441,7 +1450,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B26" s="16" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="7">
         <v>0</v>
@@ -1465,7 +1474,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C27" s="4">
         <v>0.2</v>
@@ -1489,7 +1498,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B28" s="16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C28" s="7">
         <v>0.2</v>
@@ -1541,13 +1550,13 @@
       <c r="A32" s="23"/>
       <c r="B32" s="1"/>
       <c r="C32" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="E32" s="2" t="s">
         <v>22</v>
-      </c>
-      <c r="E32" s="2" t="s">
-        <v>23</v>
       </c>
       <c r="F32" s="2" t="s">
         <v>5</v>
@@ -1563,7 +1572,7 @@
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="23"/>
       <c r="B33" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C33" s="4">
         <v>0</v>
@@ -1590,7 +1599,7 @@
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="23"/>
       <c r="B34" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C34" s="7">
         <v>0.45</v>
@@ -1617,7 +1626,7 @@
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="23"/>
       <c r="B35" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C35" s="4">
         <v>0.6</v>
@@ -1687,10 +1696,10 @@
       <c r="A39" s="23"/>
       <c r="B39" s="1"/>
       <c r="C39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>5</v>
@@ -1707,7 +1716,7 @@
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="23"/>
       <c r="B40" s="15" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="4">
         <v>0</v>
@@ -1733,7 +1742,7 @@
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="23"/>
       <c r="B41" s="16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C41" s="7">
         <v>0.4</v>
@@ -1802,10 +1811,10 @@
       <c r="A45" s="23"/>
       <c r="B45" s="1"/>
       <c r="C45" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="E45" s="2" t="s">
         <v>5</v>
@@ -1822,7 +1831,7 @@
     <row r="46" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="23"/>
       <c r="B46" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C46" s="4">
         <v>0</v>
@@ -1848,7 +1857,7 @@
     <row r="47" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="23"/>
       <c r="B47" s="16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C47" s="7">
         <v>0.05</v>
@@ -1917,10 +1926,10 @@
       <c r="A51" s="23"/>
       <c r="B51" s="1"/>
       <c r="C51" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D51" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="D51" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="E51" s="2" t="s">
         <v>5</v>
@@ -1937,7 +1946,7 @@
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="15" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C52" s="4">
         <v>0</v>
@@ -1963,7 +1972,7 @@
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C53" s="7">
         <v>0.45</v>
@@ -2048,55 +2057,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B005227-772D-45AE-8D76-50C6CC21EA45}">
   <dimension ref="B4:L19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="26.140625" customWidth="1"/>
-    <col min="3" max="3" width="16" customWidth="1"/>
-    <col min="4" max="4" width="23.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.28515625" customWidth="1"/>
-    <col min="6" max="6" width="17.140625" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" customWidth="1"/>
-    <col min="8" max="8" width="26.140625" customWidth="1"/>
-    <col min="9" max="9" width="20.140625" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" customWidth="1"/>
-    <col min="11" max="11" width="30.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.7109375" customWidth="1"/>
+    <col min="3" max="12" width="15.7109375" customWidth="1"/>
     <col min="13" max="14" width="26.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="2:12" ht="24.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:12" ht="48.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1"/>
       <c r="C5" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="G5" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="H5" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="F5" s="11" t="s">
+      <c r="I5" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="J5" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="11" t="s">
-        <v>40</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="J5" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="K5" s="11" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="L5" s="13" t="s">
         <v>5</v>
@@ -2104,7 +2104,7 @@
     </row>
     <row r="6" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B6" s="33" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="C6" s="14">
         <v>8</v>
@@ -2183,7 +2183,7 @@
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C8" s="7">
         <v>10</v>
@@ -2262,7 +2262,7 @@
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B10" s="34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10" s="14">
         <v>8</v>
@@ -2341,32 +2341,32 @@
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C14" s="32" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C15" s="32" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
       <c r="C16" s="32" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="17" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C17" s="32" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="18" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C18" s="32" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C19" s="32" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2376,5 +2376,6 @@
     <mergeCell ref="B10:B11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>